<commit_message>
Update sass question 5
</commit_message>
<xml_diff>
--- a/IS1308_SSAS_MultidimentionalAndDataMining/IS1308_SSAS_MultidimentionalAndDataMining/Question 5 Month-Day.xlsx
+++ b/IS1308_SSAS_MultidimentionalAndDataMining/IS1308_SSAS_MultidimentionalAndDataMining/Question 5 Month-Day.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="13725"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="13725"/>
   </bookViews>
   <sheets>
     <sheet name="tmp8852" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="32" r:id="rId2"/>
+    <pivotCache cacheId="54" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
   <si>
     <t>Insect Quantity</t>
   </si>
@@ -93,12 +93,6 @@
     <t>23</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
@@ -130,9 +124,6 @@
   </si>
   <si>
     <t>14</t>
-  </si>
-  <si>
-    <t>27</t>
   </si>
 </sst>
 </file>
@@ -915,263 +906,263 @@
                 <c:ptCount val="75"/>
                 <c:lvl>
                   <c:pt idx="0">
+                    <c:v>09</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>21</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>24</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>26</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>28</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>09</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>11</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>25</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>26</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>01</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="12">
+                    <c:v>04</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>07</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>08</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>13</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>23</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>25</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>28</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>04</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>18</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>21</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>25</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>26</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
                     <c:v>11</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="26">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="28">
+                    <c:v>26</c:v>
+                  </c:pt>
+                  <c:pt idx="29">
                     <c:v>29</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="30">
+                    <c:v>02</c:v>
+                  </c:pt>
+                  <c:pt idx="31">
+                    <c:v>06</c:v>
+                  </c:pt>
+                  <c:pt idx="32">
+                    <c:v>09</c:v>
+                  </c:pt>
+                  <c:pt idx="33">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="34">
+                    <c:v>24</c:v>
+                  </c:pt>
+                  <c:pt idx="35">
+                    <c:v>28</c:v>
+                  </c:pt>
+                  <c:pt idx="36">
+                    <c:v>04</c:v>
+                  </c:pt>
+                  <c:pt idx="37">
+                    <c:v>13</c:v>
+                  </c:pt>
+                  <c:pt idx="38">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="39">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="40">
+                    <c:v>19</c:v>
+                  </c:pt>
+                  <c:pt idx="41">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="42">
+                    <c:v>22</c:v>
+                  </c:pt>
+                  <c:pt idx="43">
+                    <c:v>02</c:v>
+                  </c:pt>
+                  <c:pt idx="44">
                     <c:v>03</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="45">
                     <c:v>05</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="46">
+                    <c:v>09</c:v>
+                  </c:pt>
+                  <c:pt idx="47">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="48">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="49">
+                    <c:v>19</c:v>
+                  </c:pt>
+                  <c:pt idx="50">
+                    <c:v>23</c:v>
+                  </c:pt>
+                  <c:pt idx="51">
+                    <c:v>26</c:v>
+                  </c:pt>
+                  <c:pt idx="52">
+                    <c:v>29</c:v>
+                  </c:pt>
+                  <c:pt idx="53">
+                    <c:v>02</c:v>
+                  </c:pt>
+                  <c:pt idx="54">
+                    <c:v>06</c:v>
+                  </c:pt>
+                  <c:pt idx="55">
                     <c:v>07</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>19</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>20</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>22</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>02</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>03</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>06</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>08</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>23</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>30</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>31</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>06</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>07</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>15</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>17</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>20</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>24</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>26</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>10</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>17</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>18</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>20</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>28</c:v>
-                  </c:pt>
-                  <c:pt idx="28">
-                    <c:v>31</c:v>
-                  </c:pt>
-                  <c:pt idx="29">
-                    <c:v>01</c:v>
-                  </c:pt>
-                  <c:pt idx="30">
-                    <c:v>07</c:v>
-                  </c:pt>
-                  <c:pt idx="31">
-                    <c:v>19</c:v>
-                  </c:pt>
-                  <c:pt idx="32">
-                    <c:v>04</c:v>
-                  </c:pt>
-                  <c:pt idx="33">
-                    <c:v>05</c:v>
-                  </c:pt>
-                  <c:pt idx="34">
-                    <c:v>11</c:v>
-                  </c:pt>
-                  <c:pt idx="35">
-                    <c:v>18</c:v>
-                  </c:pt>
-                  <c:pt idx="36">
-                    <c:v>19</c:v>
-                  </c:pt>
-                  <c:pt idx="37">
-                    <c:v>21</c:v>
-                  </c:pt>
-                  <c:pt idx="38">
-                    <c:v>25</c:v>
-                  </c:pt>
-                  <c:pt idx="39">
-                    <c:v>12</c:v>
-                  </c:pt>
-                  <c:pt idx="40">
-                    <c:v>13</c:v>
-                  </c:pt>
-                  <c:pt idx="41">
-                    <c:v>16</c:v>
-                  </c:pt>
-                  <c:pt idx="42">
-                    <c:v>19</c:v>
-                  </c:pt>
-                  <c:pt idx="43">
-                    <c:v>22</c:v>
-                  </c:pt>
-                  <c:pt idx="44">
-                    <c:v>31</c:v>
-                  </c:pt>
-                  <c:pt idx="45">
-                    <c:v>04</c:v>
-                  </c:pt>
-                  <c:pt idx="46">
-                    <c:v>07</c:v>
-                  </c:pt>
-                  <c:pt idx="47">
-                    <c:v>12</c:v>
-                  </c:pt>
-                  <c:pt idx="48">
-                    <c:v>14</c:v>
-                  </c:pt>
-                  <c:pt idx="49">
-                    <c:v>18</c:v>
-                  </c:pt>
-                  <c:pt idx="50">
-                    <c:v>19</c:v>
-                  </c:pt>
-                  <c:pt idx="51">
-                    <c:v>21</c:v>
-                  </c:pt>
-                  <c:pt idx="52">
-                    <c:v>24</c:v>
-                  </c:pt>
-                  <c:pt idx="53">
-                    <c:v>27</c:v>
-                  </c:pt>
-                  <c:pt idx="54">
-                    <c:v>03</c:v>
-                  </c:pt>
-                  <c:pt idx="55">
-                    <c:v>05</c:v>
                   </c:pt>
                   <c:pt idx="56">
                     <c:v>09</c:v>
                   </c:pt>
                   <c:pt idx="57">
-                    <c:v>15</c:v>
+                    <c:v>10</c:v>
                   </c:pt>
                   <c:pt idx="58">
+                    <c:v>26</c:v>
+                  </c:pt>
+                  <c:pt idx="59">
+                    <c:v>28</c:v>
+                  </c:pt>
+                  <c:pt idx="60">
+                    <c:v>06</c:v>
+                  </c:pt>
+                  <c:pt idx="61">
+                    <c:v>09</c:v>
+                  </c:pt>
+                  <c:pt idx="62">
+                    <c:v>19</c:v>
+                  </c:pt>
+                  <c:pt idx="63">
+                    <c:v>24</c:v>
+                  </c:pt>
+                  <c:pt idx="64">
+                    <c:v>28</c:v>
+                  </c:pt>
+                  <c:pt idx="65">
+                    <c:v>01</c:v>
+                  </c:pt>
+                  <c:pt idx="66">
+                    <c:v>05</c:v>
+                  </c:pt>
+                  <c:pt idx="67">
+                    <c:v>18</c:v>
+                  </c:pt>
+                  <c:pt idx="68">
+                    <c:v>24</c:v>
+                  </c:pt>
+                  <c:pt idx="69">
+                    <c:v>29</c:v>
+                  </c:pt>
+                  <c:pt idx="70">
+                    <c:v>07</c:v>
+                  </c:pt>
+                  <c:pt idx="71">
                     <c:v>17</c:v>
                   </c:pt>
-                  <c:pt idx="59">
+                  <c:pt idx="72">
                     <c:v>22</c:v>
                   </c:pt>
-                  <c:pt idx="60">
-                    <c:v>23</c:v>
-                  </c:pt>
-                  <c:pt idx="61">
+                  <c:pt idx="73">
                     <c:v>24</c:v>
                   </c:pt>
-                  <c:pt idx="62">
-                    <c:v>25</c:v>
-                  </c:pt>
-                  <c:pt idx="63">
-                    <c:v>02</c:v>
-                  </c:pt>
-                  <c:pt idx="64">
-                    <c:v>05</c:v>
-                  </c:pt>
-                  <c:pt idx="65">
-                    <c:v>12</c:v>
-                  </c:pt>
-                  <c:pt idx="66">
-                    <c:v>15</c:v>
-                  </c:pt>
-                  <c:pt idx="67">
-                    <c:v>20</c:v>
-                  </c:pt>
-                  <c:pt idx="68">
-                    <c:v>23</c:v>
-                  </c:pt>
-                  <c:pt idx="69">
-                    <c:v>30</c:v>
-                  </c:pt>
-                  <c:pt idx="70">
-                    <c:v>12</c:v>
-                  </c:pt>
-                  <c:pt idx="71">
-                    <c:v>14</c:v>
-                  </c:pt>
-                  <c:pt idx="72">
-                    <c:v>18</c:v>
-                  </c:pt>
-                  <c:pt idx="73">
-                    <c:v>19</c:v>
-                  </c:pt>
                   <c:pt idx="74">
-                    <c:v>31</c:v>
+                    <c:v>26</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>01</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="7">
                     <c:v>02</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="11">
                     <c:v>03</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="19">
                     <c:v>04</c:v>
                   </c:pt>
-                  <c:pt idx="23">
+                  <c:pt idx="25">
                     <c:v>05</c:v>
                   </c:pt>
-                  <c:pt idx="29">
+                  <c:pt idx="30">
                     <c:v>06</c:v>
                   </c:pt>
-                  <c:pt idx="32">
+                  <c:pt idx="36">
                     <c:v>07</c:v>
                   </c:pt>
-                  <c:pt idx="39">
+                  <c:pt idx="43">
                     <c:v>08</c:v>
                   </c:pt>
-                  <c:pt idx="45">
+                  <c:pt idx="53">
                     <c:v>09</c:v>
                   </c:pt>
-                  <c:pt idx="54">
+                  <c:pt idx="60">
                     <c:v>10</c:v>
                   </c:pt>
-                  <c:pt idx="63">
+                  <c:pt idx="65">
                     <c:v>11</c:v>
                   </c:pt>
                   <c:pt idx="70">
@@ -1188,145 +1179,145 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="75"/>
                 <c:pt idx="0">
-                  <c:v>201</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>914</c:v>
+                  <c:v>183</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>143</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>193</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>302</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>176</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>145</c:v>
+                  <c:v>165</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>183</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>165</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>196</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>62</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>123</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>159</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>173</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>119</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>190</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>233</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>104</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="42">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>68</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>502</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>173</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>186</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>181</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>61</c:v>
-                </c:pt>
                 <c:pt idx="43">
-                  <c:v>154</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>92</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>100</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>410</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>42</c:v>
@@ -1335,82 +1326,82 @@
                   <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>72</c:v>
+                  <c:v>103</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>87</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>220</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>100</c:v>
+                  <c:v>531</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>365</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>103</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>18</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>166</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>85</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>96</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>180</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>33</c:v>
+                  <c:v>722</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>55</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>39</c:v>
+                  <c:v>438</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>484</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>72</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>134</c:v>
+                  <c:v>178</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>438</c:v>
+                  <c:v>258</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>238</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>83</c:v>
+                  <c:v>914</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>24</c:v>
+                  <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>27</c:v>
+                  <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>95</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>89</c:v>
+                  <c:v>302</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>258</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2180,69 +2171,67 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PC" refreshedDate="44041.079901620367" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="PC" refreshedDate="44041.563691782409" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
-    <cacheField name="[Measures].[Insect Quantity]" caption="Insect Quantity" numFmtId="0" hierarchy="36" level="32767"/>
-    <cacheField name="[Time].[Month Formated].[Month Formated]" caption="Month Formated" numFmtId="0" hierarchy="25" level="1">
+    <cacheField name="[Measures].[Insect Quantity]" caption="Insect Quantity" numFmtId="0" hierarchy="39" level="32767"/>
+    <cacheField name="[Time].[Lunar Month Formated].[Lunar Month Formated]" caption="Lunar Month Formated" numFmtId="0" hierarchy="24" level="1">
       <sharedItems count="12">
-        <s v="[Time].[Month Formated].&amp;[01]" c="01"/>
-        <s v="[Time].[Month Formated].&amp;[02]" c="02"/>
-        <s v="[Time].[Month Formated].&amp;[03]" c="03"/>
-        <s v="[Time].[Month Formated].&amp;[04]" c="04"/>
-        <s v="[Time].[Month Formated].&amp;[05]" c="05"/>
-        <s v="[Time].[Month Formated].&amp;[06]" c="06"/>
-        <s v="[Time].[Month Formated].&amp;[07]" c="07"/>
-        <s v="[Time].[Month Formated].&amp;[08]" c="08"/>
-        <s v="[Time].[Month Formated].&amp;[09]" c="09"/>
-        <s v="[Time].[Month Formated].&amp;[10]" c="10"/>
-        <s v="[Time].[Month Formated].&amp;[11]" c="11"/>
-        <s v="[Time].[Month Formated].&amp;[12]" c="12"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[01]" c="01"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[02]" c="02"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[03]" c="03"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[04]" c="04"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[05]" c="05"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[06]" c="06"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[07]" c="07"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[08]" c="08"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[09]" c="09"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[10]" c="10"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[11]" c="11"/>
+        <s v="[Time].[Lunar Month Formated].&amp;[12]" c="12"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="[Time].[Day Formated].[Day Formated]" caption="Day Formated" numFmtId="0" hierarchy="20" level="1">
-      <sharedItems count="31">
-        <s v="[Time].[Day Formated].&amp;[01]" c="01"/>
-        <s v="[Time].[Day Formated].&amp;[02]" c="02"/>
-        <s v="[Time].[Day Formated].&amp;[03]" c="03"/>
-        <s v="[Time].[Day Formated].&amp;[04]" c="04"/>
-        <s v="[Time].[Day Formated].&amp;[05]" c="05"/>
-        <s v="[Time].[Day Formated].&amp;[06]" c="06"/>
-        <s v="[Time].[Day Formated].&amp;[07]" c="07"/>
-        <s v="[Time].[Day Formated].&amp;[08]" c="08"/>
-        <s v="[Time].[Day Formated].&amp;[09]" c="09"/>
-        <s v="[Time].[Day Formated].&amp;[10]" c="10"/>
-        <s v="[Time].[Day Formated].&amp;[11]" c="11"/>
-        <s v="[Time].[Day Formated].&amp;[12]" c="12"/>
-        <s v="[Time].[Day Formated].&amp;[13]" c="13"/>
-        <s v="[Time].[Day Formated].&amp;[14]" c="14"/>
-        <s v="[Time].[Day Formated].&amp;[15]" c="15"/>
-        <s v="[Time].[Day Formated].&amp;[16]" c="16"/>
-        <s v="[Time].[Day Formated].&amp;[17]" c="17"/>
-        <s v="[Time].[Day Formated].&amp;[18]" c="18"/>
-        <s v="[Time].[Day Formated].&amp;[19]" c="19"/>
-        <s v="[Time].[Day Formated].&amp;[20]" c="20"/>
-        <s v="[Time].[Day Formated].&amp;[21]" c="21"/>
-        <s v="[Time].[Day Formated].&amp;[22]" c="22"/>
-        <s v="[Time].[Day Formated].&amp;[23]" c="23"/>
-        <s v="[Time].[Day Formated].&amp;[24]" c="24"/>
-        <s v="[Time].[Day Formated].&amp;[25]" c="25"/>
-        <s v="[Time].[Day Formated].&amp;[26]" c="26"/>
-        <s v="[Time].[Day Formated].&amp;[27]" c="27"/>
-        <s v="[Time].[Day Formated].&amp;[28]" c="28"/>
-        <s v="[Time].[Day Formated].&amp;[29]" c="29"/>
-        <s v="[Time].[Day Formated].&amp;[30]" c="30"/>
-        <s v="[Time].[Day Formated].&amp;[31]" c="31"/>
+    <cacheField name="[Time].[Lunnar Day Formated].[Lunnar Day Formated]" caption="Lunnar Day Formated" numFmtId="0" hierarchy="26" level="1">
+      <sharedItems count="28">
+        <s v="[Time].[Lunnar Day Formated].&amp;[01]" c="01"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[02]" c="02"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[03]" c="03"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[04]" c="04"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[05]" c="05"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[06]" c="06"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[07]" c="07"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[08]" c="08"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[09]" c="09"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[10]" c="10"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[11]" c="11"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[12]" c="12"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[13]" c="13"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[14]" c="14"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[15]" c="15"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[16]" c="16"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[17]" c="17"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[18]" c="18"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[19]" c="19"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[20]" c="20"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[21]" c="21"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[22]" c="22"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[23]" c="23"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[24]" c="24"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[25]" c="25"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[26]" c="26"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[28]" c="28"/>
+        <s v="[Time].[Lunnar Day Formated].&amp;[29]" c="29"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
-  <cacheHierarchies count="40">
+  <cacheHierarchies count="43">
     <cacheHierarchy uniqueName="[Facts].[Approximate Size]" caption="Approximate Size" attribute="1" defaultMemberUniqueName="[Facts].[Approximate Size].[All]" allUniqueName="[Facts].[Approximate Size].[All]" dimensionUniqueName="[Facts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Facts].[Checked Insect Line]" caption="Checked Insect Line" attribute="1" defaultMemberUniqueName="[Facts].[Checked Insect Line].[All]" allUniqueName="[Facts].[Checked Insect Line].[All]" dimensionUniqueName="[Facts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Facts].[Ecosystem]" caption="Ecosystem" attribute="1" defaultMemberUniqueName="[Facts].[Ecosystem].[All]" allUniqueName="[Facts].[Ecosystem].[All]" dimensionUniqueName="[Facts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Facts].[Insect Age]" caption="Insect Age" attribute="1" defaultMemberUniqueName="[Facts].[Insect Age].[All]" allUniqueName="[Facts].[Insect Age].[All]" dimensionUniqueName="[Facts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Facts].[Insect Quantity]" caption="Insect Quantity" attribute="1" defaultMemberUniqueName="[Facts].[Insect Quantity].[All]" allUniqueName="[Facts].[Insect Quantity].[All]" dimensionUniqueName="[Facts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Facts].[Pesticides Level]" caption="Pesticides Level" attribute="1" defaultMemberUniqueName="[Facts].[Pesticides Level].[All]" allUniqueName="[Facts].[Pesticides Level].[All]" dimensionUniqueName="[Facts]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Facts].[Pesticides Level Formated]" caption="Pesticides Level Formated" attribute="1" defaultMemberUniqueName="[Facts].[Pesticides Level Formated].[All]" allUniqueName="[Facts].[Pesticides Level Formated].[All]" dimensionUniqueName="[Facts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Facts].[Time Key]" caption="Time Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Facts].[Time Key].[All]" allUniqueName="[Facts].[Time Key].[All]" dimensionUniqueName="[Facts]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Farmer].[End Date]" caption="End Date" attribute="1" defaultMemberUniqueName="[Farmer].[End Date].[All]" allUniqueName="[Farmer].[End Date].[All]" dimensionUniqueName="[Farmer]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Farmer].[Farmer Address]" caption="Farmer Address" attribute="1" defaultMemberUniqueName="[Farmer].[Farmer Address].[All]" allUniqueName="[Farmer].[Farmer Address].[All]" dimensionUniqueName="[Farmer]" displayFolder="" count="0" unbalanced="0"/>
@@ -2257,22 +2246,24 @@
     <cacheHierarchy uniqueName="[Insect].[Sub Kind]" caption="Sub Kind" attribute="1" defaultMemberUniqueName="[Insect].[Sub Kind].[All]" allUniqueName="[Insect].[Sub Kind].[All]" dimensionUniqueName="[Insect]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Insect].[Type]" caption="Type" attribute="1" defaultMemberUniqueName="[Insect].[Type].[All]" allUniqueName="[Insect].[Type].[All]" dimensionUniqueName="[Insect]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Time].[Day]" caption="Day" attribute="1" defaultMemberUniqueName="[Time].[Day].[All]" allUniqueName="[Time].[Day].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Time].[Day Formated]" caption="Day Formated" attribute="1" defaultMemberUniqueName="[Time].[Day Formated].[All]" allUniqueName="[Time].[Day Formated].[All]" dimensionUniqueName="[Time]" displayFolder="" count="2" unbalanced="0">
+    <cacheHierarchy uniqueName="[Time].[Day Formated]" caption="Day Formated" attribute="1" defaultMemberUniqueName="[Time].[Day Formated].[All]" allUniqueName="[Time].[Day Formated].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Time].[Lunar Day]" caption="Lunar Day" attribute="1" defaultMemberUniqueName="[Time].[Lunar Day].[All]" allUniqueName="[Time].[Lunar Day].[All]" dimensionUniqueName="[Time]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Time].[Lunar Month]" caption="Lunar Month" attribute="1" defaultMemberUniqueName="[Time].[Lunar Month].[All]" allUniqueName="[Time].[Lunar Month].[All]" dimensionUniqueName="[Time]" displayFolder="" count="2" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Time].[Lunar Month Formated]" caption="Lunar Month Formated" attribute="1" defaultMemberUniqueName="[Time].[Lunar Month Formated].[All]" allUniqueName="[Time].[Lunar Month Formated].[All]" dimensionUniqueName="[Time]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Time].[Lunar Year]" caption="Lunar Year" attribute="1" defaultMemberUniqueName="[Time].[Lunar Year].[All]" allUniqueName="[Time].[Lunar Year].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Time].[Lunnar Day Formated]" caption="Lunnar Day Formated" attribute="1" defaultMemberUniqueName="[Time].[Lunnar Day Formated].[All]" allUniqueName="[Time].[Lunnar Day Formated].[All]" dimensionUniqueName="[Time]" displayFolder="" count="2" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
         <fieldUsage x="2"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Time].[Lunar Day]" caption="Lunar Day" attribute="1" defaultMemberUniqueName="[Time].[Lunar Day].[All]" allUniqueName="[Time].[Lunar Day].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Time].[Lunar Month]" caption="Lunar Month" attribute="1" defaultMemberUniqueName="[Time].[Lunar Month].[All]" allUniqueName="[Time].[Lunar Month].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Time].[Lunar Year]" caption="Lunar Year" attribute="1" defaultMemberUniqueName="[Time].[Lunar Year].[All]" allUniqueName="[Time].[Lunar Year].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Time].[Month]" caption="Month" attribute="1" defaultMemberUniqueName="[Time].[Month].[All]" allUniqueName="[Time].[Month].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Time].[Month Formated]" caption="Month Formated" attribute="1" defaultMemberUniqueName="[Time].[Month Formated].[All]" allUniqueName="[Time].[Month Formated].[All]" dimensionUniqueName="[Time]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Time].[Month Formated]" caption="Month Formated" attribute="1" defaultMemberUniqueName="[Time].[Month Formated].[All]" allUniqueName="[Time].[Month Formated].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Time].[Time Key]" caption="Time Key" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Time].[Time Key].[All]" allUniqueName="[Time].[Time Key].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Time].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Time].[Year].[All]" allUniqueName="[Time].[Year].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Time].[Year Month]" caption="Year Month" attribute="1" defaultMemberUniqueName="[Time].[Year Month].[All]" allUniqueName="[Time].[Year Month].[All]" dimensionUniqueName="[Time]" displayFolder="" count="0" unbalanced="0"/>
@@ -2320,7 +2311,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="32" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
   <location ref="A1:B89" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -2342,7 +2333,7 @@
       </items>
     </pivotField>
     <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
-      <items count="32">
+      <items count="29">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -2371,9 +2362,6 @@
         <item x="25"/>
         <item x="26"/>
         <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2387,79 +2375,85 @@
       <x/>
     </i>
     <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="28"/>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
     </i>
     <i>
       <x v="1"/>
     </i>
     <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
     </i>
     <i>
       <x v="2"/>
     </i>
     <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
     </i>
     <i r="1">
       <x v="7"/>
     </i>
     <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
       <x v="22"/>
     </i>
     <i r="1">
-      <x v="29"/>
-    </i>
-    <i r="1">
-      <x v="30"/>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
     </i>
     <i>
       <x v="3"/>
     </i>
     <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="23"/>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
     </i>
     <i r="1">
       <x v="25"/>
@@ -2468,34 +2462,40 @@
       <x v="4"/>
     </i>
     <i r="1">
-      <x v="9"/>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
     </i>
     <i r="1">
       <x v="16"/>
     </i>
     <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
+      <x v="25"/>
     </i>
     <i r="1">
       <x v="27"/>
-    </i>
-    <i r="1">
-      <x v="30"/>
     </i>
     <i>
       <x v="5"/>
     </i>
     <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
     </i>
     <i>
       <x v="6"/>
@@ -2504,31 +2504,40 @@
       <x v="3"/>
     </i>
     <i r="1">
-      <x v="4"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
     </i>
     <i r="1">
       <x v="18"/>
     </i>
     <i r="1">
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="24"/>
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
     </i>
     <i>
       <x v="7"/>
     </i>
     <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="12"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
     </i>
     <i r="1">
       <x v="15"/>
@@ -2537,37 +2546,34 @@
       <x v="18"/>
     </i>
     <i r="1">
-      <x v="21"/>
-    </i>
-    <i r="1">
-      <x v="30"/>
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
     </i>
     <i>
       <x v="8"/>
     </i>
     <i r="1">
-      <x v="3"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
     </i>
     <i r="1">
       <x v="6"/>
     </i>
     <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="20"/>
-    </i>
-    <i r="1">
-      <x v="23"/>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
     </i>
     <i r="1">
       <x v="26"/>
@@ -2576,73 +2582,55 @@
       <x v="9"/>
     </i>
     <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
+      <x v="5"/>
     </i>
     <i r="1">
       <x v="8"/>
     </i>
     <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="16"/>
-    </i>
-    <i r="1">
-      <x v="21"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
+      <x v="18"/>
     </i>
     <i r="1">
       <x v="23"/>
     </i>
     <i r="1">
-      <x v="24"/>
+      <x v="26"/>
     </i>
     <i>
       <x v="10"/>
     </i>
     <i r="1">
-      <x v="1"/>
+      <x/>
     </i>
     <i r="1">
       <x v="4"/>
     </i>
     <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="14"/>
-    </i>
-    <i r="1">
-      <x v="19"/>
-    </i>
-    <i r="1">
-      <x v="22"/>
-    </i>
-    <i r="1">
-      <x v="29"/>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
     </i>
     <i>
       <x v="11"/>
     </i>
     <i r="1">
-      <x v="11"/>
-    </i>
-    <i r="1">
-      <x v="13"/>
-    </i>
-    <i r="1">
-      <x v="17"/>
-    </i>
-    <i r="1">
-      <x v="18"/>
-    </i>
-    <i r="1">
-      <x v="30"/>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
     </i>
     <i t="grand">
       <x/>
@@ -2665,7 +2653,10 @@
       </pivotArea>
     </chartFormat>
   </chartFormats>
-  <pivotHierarchies count="40">
+  <pivotHierarchies count="43">
+    <pivotHierarchy/>
+    <pivotHierarchy/>
+    <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -2709,8 +2700,8 @@
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <rowHierarchiesUsage count="2">
-    <rowHierarchyUsage hierarchyUsage="25"/>
-    <rowHierarchyUsage hierarchyUsage="20"/>
+    <rowHierarchyUsage hierarchyUsage="24"/>
+    <rowHierarchyUsage hierarchyUsage="26"/>
   </rowHierarchiesUsage>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -3008,199 +2999,199 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1258</v>
+        <v>906</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>201</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
-        <v>914</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>3</v>
+      <c r="A6" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B6" s="1">
-        <v>1055</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1">
-        <v>193</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
-        <v>302</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1">
-        <v>176</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
+      <c r="A10" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B10" s="1">
-        <v>56</v>
+        <v>488</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>145</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
-        <v>183</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>4</v>
+      <c r="A13" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B13" s="1">
-        <v>1074</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1">
-        <v>165</v>
+        <v>190</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="1">
-        <v>196</v>
+        <v>908</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B16" s="1">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1">
-        <v>123</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1">
-        <v>159</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1">
-        <v>250</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
         <v>21</v>
-      </c>
-      <c r="B20" s="1">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1">
-        <v>737</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1">
-        <v>41</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1">
-        <v>190</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>22</v>
+      <c r="A24" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B24" s="1">
-        <v>233</v>
+        <v>942</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B25" s="1">
-        <v>104</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B26" s="1">
-        <v>108</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -3208,151 +3199,151 @@
         <v>24</v>
       </c>
       <c r="B27" s="1">
-        <v>27</v>
+        <v>570</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1">
-        <v>34</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>6</v>
+      <c r="A29" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="B29" s="1">
-        <v>908</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1">
-        <v>68</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>23</v>
+      <c r="A31" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B31" s="1">
-        <v>42</v>
+        <v>451</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B32" s="1">
-        <v>97</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1">
-        <v>77</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B34" s="1">
-        <v>502</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B35" s="1">
-        <v>122</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="1">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="1">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>2</v>
-      </c>
       <c r="B37" s="1">
-        <v>44</v>
+        <v>512</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B38" s="1">
-        <v>144</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B39" s="1">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>8</v>
+      <c r="A40" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B40" s="1">
-        <v>660</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B41" s="1">
-        <v>8</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B42" s="1">
-        <v>61</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B43" s="1">
-        <v>173</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>26</v>
+      <c r="A44" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="B44" s="1">
-        <v>1</v>
+        <v>791</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B45" s="1">
-        <v>186</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -3360,7 +3351,7 @@
         <v>28</v>
       </c>
       <c r="B46" s="1">
-        <v>181</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -3368,287 +3359,287 @@
         <v>29</v>
       </c>
       <c r="B47" s="1">
-        <v>50</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>9</v>
+      <c r="A48" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B48" s="1">
-        <v>548</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B49" s="1">
-        <v>92</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B50" s="1">
-        <v>52</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B51" s="1">
-        <v>97</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>16</v>
+      <c r="A52" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B52" s="1">
-        <v>61</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B53" s="1">
-        <v>154</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B54" s="1">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>10</v>
+      <c r="A55" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B55" s="1">
-        <v>1489</v>
+        <v>220</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B56" s="1">
-        <v>100</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B57" s="1">
-        <v>410</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B58" s="1">
-        <v>42</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="B59" s="1">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B60" s="1">
-        <v>72</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B61" s="1">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B62" s="1">
-        <v>220</v>
+        <v>531</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>24</v>
+      <c r="A63" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B63" s="1">
-        <v>100</v>
+        <v>527</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B64" s="1">
-        <v>365</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
-        <v>11</v>
+      <c r="A65" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B65" s="1">
-        <v>742</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B66" s="1">
-        <v>6</v>
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B67" s="1">
-        <v>103</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B68" s="1">
-        <v>18</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B69" s="1">
-        <v>166</v>
+        <v>180</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B70" s="1">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
-        <v>18</v>
+      <c r="A71" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B71" s="1">
-        <v>96</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B72" s="1">
-        <v>180</v>
+        <v>39</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B73" s="1">
-        <v>33</v>
+        <v>722</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B74" s="1">
-        <v>55</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>12</v>
+      <c r="A75" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B75" s="1">
-        <v>1488</v>
+        <v>438</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B76" s="1">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>6</v>
+      <c r="A77" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B77" s="1">
-        <v>484</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B78" s="1">
-        <v>72</v>
+        <v>27</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B79" s="1">
-        <v>134</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B80" s="1">
-        <v>438</v>
+        <v>258</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B81" s="1">
-        <v>238</v>
+        <v>89</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B82" s="1">
-        <v>83</v>
+        <v>914</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -3656,47 +3647,47 @@
         <v>13</v>
       </c>
       <c r="B83" s="1">
-        <v>493</v>
+        <v>874</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B84" s="1">
-        <v>24</v>
+        <v>201</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B85" s="1">
-        <v>27</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B86" s="1">
-        <v>95</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B87" s="1">
-        <v>89</v>
+        <v>302</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B88" s="1">
-        <v>258</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>